<commit_message>
Routes checked and verified
</commit_message>
<xml_diff>
--- a/backend/test-users.xlsx
+++ b/backend/test-users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD147E6-9920-4A1A-9DA9-4976B68A34D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD0BFBF-7578-4D2E-823F-C3BBBE4950CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>studentId</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>test1234</t>
+  </si>
+  <si>
+    <t>CB00000</t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +472,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>

</xml_diff>

<commit_message>
Updated the profile page to display more information and statistics
</commit_message>
<xml_diff>
--- a/backend/test-users.xlsx
+++ b/backend/test-users.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD0BFBF-7578-4D2E-823F-C3BBBE4950CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAD92DC-3327-403A-9E5B-D1843770EC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>studentId</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>CB00000</t>
+  </si>
+  <si>
+    <t>CB23002</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,6 +483,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>12345678</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>

</xml_diff>

<commit_message>
Fixed the My clubs section
</commit_message>
<xml_diff>
--- a/backend/test-users.xlsx
+++ b/backend/test-users.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAD92DC-3327-403A-9E5B-D1843770EC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B75262-85AE-4D12-ABF5-E37FB578DE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>studentId</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>CB23002</t>
+  </si>
+  <si>
+    <t>CB24190</t>
+  </si>
+  <si>
+    <t>TEST11111</t>
+  </si>
+  <si>
+    <t>CB21130</t>
   </si>
 </sst>
 </file>
@@ -424,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,6 +500,22 @@
         <v>12345678</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>

</xml_diff>